<commit_message>
feat: se añade lógica cargue masivo órdenes de compra
</commit_message>
<xml_diff>
--- a/apps/static/cargues_masivos/ejemplo_ordenes_compra.xlsx
+++ b/apps/static/cargues_masivos/ejemplo_ordenes_compra.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SINTRA\apps\templates\cargues_masivos\ejemplos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SINTRA\apps\static\cargues_masivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902EA54F-F8A2-4823-A52F-16F2D225BCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438D98CF-1614-4DF5-8C93-03DA6BBA6999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>ORDENES_COMPRA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t>CÓDIGO OC</t>
+  </si>
+  <si>
+    <t>FECHA SOLICITUD</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>PROYECTO</t>
+  </si>
+  <si>
+    <t>PRODUCTO</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN EN OC</t>
+  </si>
+  <si>
+    <t>OCAM-63-2021-115</t>
+  </si>
+  <si>
+    <t>deltec</t>
+  </si>
+  <si>
+    <t>AIR-E - ACTUACIONES MASIVAS</t>
+  </si>
+  <si>
+    <t>CI1-U</t>
+  </si>
+  <si>
+    <t>CINTURON IGNIFUGO AZUL REY DIELECTRICO AIR-E</t>
+  </si>
+  <si>
+    <t>OCAM-57-2021-115</t>
+  </si>
+  <si>
+    <t>CIH1-XXL</t>
+  </si>
+  <si>
+    <t>CAMISA IGNIFUGO AZUL REY CELESTE HOMBRE AIR-E</t>
+  </si>
+  <si>
+    <t>DELTEC</t>
+  </si>
+  <si>
+    <t>CIH1-L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,13 +90,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +125,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,17 +416,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" customWidth="1"/>
+    <col min="6" max="6" width="56" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44551</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44550</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44550</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>